<commit_message>
RELACION DE MICROSERVICIOS EN EL FORMATO SUGERIDO
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/MICROSERVICIOS.xlsx
+++ b/DOCUMENTACION/MICROSERVICIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\localCode\MINTIC_CICLO4\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76E65B6-F9BD-4589-8228-374785CC5C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD550F3-7029-4A21-A30B-3BE3911DFE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B0264229-AF5F-4166-AE28-8EBCC666E9AB}"/>
   </bookViews>
@@ -377,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -401,15 +401,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -738,524 +737,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5629C3C8-928B-472F-A7BE-66F422D71C56}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="76.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>10</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>13</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>43</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>16</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="F28" s="16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>17</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="8" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="17"/>
+      <c r="C31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>57</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="F32" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+    <row r="36" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>19</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="E36" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="F36" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>64</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>65</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>22</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="F38" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>22</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>67</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>22</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="F39" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="16"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{65019BF7-9D28-4B41-9FD0-9F5572C3EE7F}"/>
-    <hyperlink ref="E4:E8" r:id="rId2" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{1CC698EC-3510-4083-9755-C6143C6D2AAB}"/>
-    <hyperlink ref="E13" r:id="rId3" xr:uid="{2E6E4960-3C18-4B03-ABD2-5B7688F4FE8C}"/>
-    <hyperlink ref="E16" r:id="rId4" xr:uid="{0FE900B7-686F-4678-9622-84752D5526D2}"/>
-    <hyperlink ref="E26" r:id="rId5" xr:uid="{9D883BD7-31EE-4A26-9680-DF8CB1273098}"/>
-    <hyperlink ref="E25" r:id="rId6" xr:uid="{DA298F45-C5DC-4624-BA36-8FC502D01746}"/>
-    <hyperlink ref="E27:E29" r:id="rId7" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{0B7F858B-8774-4F43-8908-775D35E9A024}"/>
-    <hyperlink ref="E32" r:id="rId8" xr:uid="{B77F7194-C584-4841-94DB-717846DD0196}"/>
-    <hyperlink ref="E36:E39" r:id="rId9" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{C153E21C-4113-408A-9960-1BF411D13CC7}"/>
-    <hyperlink ref="E8" r:id="rId10" xr:uid="{0063A8DA-A993-4393-85B8-352DA9FD860F}"/>
-    <hyperlink ref="E4" r:id="rId11" xr:uid="{A1E0651C-0D99-427E-9F8C-C467E0C4A010}"/>
-    <hyperlink ref="E5" r:id="rId12" xr:uid="{3886DD18-E946-4C0B-9A27-50B8773ECDD1}"/>
-    <hyperlink ref="E6" r:id="rId13" xr:uid="{2A372D1C-3234-486A-96B2-E2D002EF7BDE}"/>
-    <hyperlink ref="E7" r:id="rId14" xr:uid="{ED2433EA-153B-494B-BEAD-B53EFCC6763F}"/>
-    <hyperlink ref="E19" r:id="rId15" xr:uid="{67F7CE5B-2F59-4AFA-9423-CF1B8760DE24}"/>
-    <hyperlink ref="E20" r:id="rId16" xr:uid="{71B89D32-89EA-47ED-A55E-69BD1EBD9BB2}"/>
-    <hyperlink ref="E21" r:id="rId17" xr:uid="{A83E858F-6E51-4F0D-877E-5D55A27A6624}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{D89DC6A9-C17C-4C81-9C4E-718C0F5BD3C0}"/>
-    <hyperlink ref="E27" r:id="rId19" xr:uid="{63574C11-2616-458F-80BE-B4E904A6678F}"/>
-    <hyperlink ref="E28" r:id="rId20" xr:uid="{4B99C02C-5C8D-47C8-BDF9-517CBE94A24C}"/>
-    <hyperlink ref="E29" r:id="rId21" xr:uid="{0226A9CA-1BF1-4EB9-A105-57E2E63146B6}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{65019BF7-9D28-4B41-9FD0-9F5572C3EE7F}"/>
+    <hyperlink ref="F4:F8" r:id="rId2" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{1CC698EC-3510-4083-9755-C6143C6D2AAB}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{2E6E4960-3C18-4B03-ABD2-5B7688F4FE8C}"/>
+    <hyperlink ref="F16" r:id="rId4" xr:uid="{0FE900B7-686F-4678-9622-84752D5526D2}"/>
+    <hyperlink ref="F26" r:id="rId5" xr:uid="{9D883BD7-31EE-4A26-9680-DF8CB1273098}"/>
+    <hyperlink ref="F25" r:id="rId6" xr:uid="{DA298F45-C5DC-4624-BA36-8FC502D01746}"/>
+    <hyperlink ref="F27:F29" r:id="rId7" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{0B7F858B-8774-4F43-8908-775D35E9A024}"/>
+    <hyperlink ref="F32" r:id="rId8" xr:uid="{B77F7194-C584-4841-94DB-717846DD0196}"/>
+    <hyperlink ref="F36:F39" r:id="rId9" display="https://[URL_SERVER]/votaciones/getUsuario/id=?" xr:uid="{C153E21C-4113-408A-9960-1BF411D13CC7}"/>
+    <hyperlink ref="F8" r:id="rId10" xr:uid="{0063A8DA-A993-4393-85B8-352DA9FD860F}"/>
+    <hyperlink ref="F4" r:id="rId11" xr:uid="{A1E0651C-0D99-427E-9F8C-C467E0C4A010}"/>
+    <hyperlink ref="F5" r:id="rId12" xr:uid="{3886DD18-E946-4C0B-9A27-50B8773ECDD1}"/>
+    <hyperlink ref="F6" r:id="rId13" xr:uid="{2A372D1C-3234-486A-96B2-E2D002EF7BDE}"/>
+    <hyperlink ref="F7" r:id="rId14" xr:uid="{ED2433EA-153B-494B-BEAD-B53EFCC6763F}"/>
+    <hyperlink ref="F19" r:id="rId15" xr:uid="{67F7CE5B-2F59-4AFA-9423-CF1B8760DE24}"/>
+    <hyperlink ref="F20" r:id="rId16" xr:uid="{71B89D32-89EA-47ED-A55E-69BD1EBD9BB2}"/>
+    <hyperlink ref="F21" r:id="rId17" xr:uid="{A83E858F-6E51-4F0D-877E-5D55A27A6624}"/>
+    <hyperlink ref="F22" r:id="rId18" xr:uid="{D89DC6A9-C17C-4C81-9C4E-718C0F5BD3C0}"/>
+    <hyperlink ref="F27" r:id="rId19" xr:uid="{63574C11-2616-458F-80BE-B4E904A6678F}"/>
+    <hyperlink ref="F28" r:id="rId20" xr:uid="{4B99C02C-5C8D-47C8-BDF9-517CBE94A24C}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{0226A9CA-1BF1-4EB9-A105-57E2E63146B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>

</xml_diff>